<commit_message>
Add IGHE and IGKC, remove SDC1, as PC markers
</commit_message>
<xml_diff>
--- a/analysis/summary/immune-cell-markers.xlsx
+++ b/analysis/summary/immune-cell-markers.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/work/sage/deconvolution/Tumor-Deconvolution-Challenge/analysis/summary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whitebr/work/sage/Tumor-Deconvolution-Challenge/analysis/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78499A0-C17F-0C40-82FB-F1F8E14EF2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="460" windowWidth="24640" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="-36760" yWindow="1620" windowWidth="24640" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>cell.type</t>
   </si>
@@ -134,9 +135,6 @@
     <t>MZB1</t>
   </si>
   <si>
-    <t>SDC1</t>
-  </si>
-  <si>
     <t>Tregs</t>
   </si>
   <si>
@@ -198,12 +196,18 @@
   </si>
   <si>
     <t>CD274</t>
+  </si>
+  <si>
+    <t>IGKC</t>
+  </si>
+  <si>
+    <t>IGHE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -272,6 +276,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -539,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,10 +565,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -609,15 +616,15 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -625,7 +632,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -633,31 +640,31 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -665,31 +672,31 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -697,7 +704,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -705,15 +712,15 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -721,7 +728,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -729,15 +736,15 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -753,15 +760,15 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -769,7 +776,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -777,7 +784,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -785,63 +792,71 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
         <v>46</v>
-      </c>
-      <c r="B36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Plasma Cell markers
</commit_message>
<xml_diff>
--- a/analysis/summary/immune-cell-markers.xlsx
+++ b/analysis/summary/immune-cell-markers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whitebr/work/sage/Tumor-Deconvolution-Challenge/analysis/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78499A0-C17F-0C40-82FB-F1F8E14EF2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A837670-8298-5E44-BFCF-8FA6CDA82258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36760" yWindow="1620" windowWidth="24640" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28380" yWindow="2400" windowWidth="24640" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>cell.type</t>
   </si>
@@ -129,12 +129,6 @@
     <t>TCL1A</t>
   </si>
   <si>
-    <t>Plasma cells</t>
-  </si>
-  <si>
-    <t>MZB1</t>
-  </si>
-  <si>
     <t>Tregs</t>
   </si>
   <si>
@@ -196,12 +190,6 @@
   </si>
   <si>
     <t>CD274</t>
-  </si>
-  <si>
-    <t>IGKC</t>
-  </si>
-  <si>
-    <t>IGHE</t>
   </si>
 </sst>
 </file>
@@ -547,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,10 +553,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -605,170 +593,170 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -776,87 +764,63 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise immune cell markers
</commit_message>
<xml_diff>
--- a/analysis/summary/immune-cell-markers.xlsx
+++ b/analysis/summary/immune-cell-markers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whitebr/work/sage/Tumor-Deconvolution-Challenge/analysis/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A837670-8298-5E44-BFCF-8FA6CDA82258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE6B45F-9DA9-D748-8BF1-FB1C0964E89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="2400" windowWidth="24640" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17160" yWindow="6120" windowWidth="24640" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>cell.type</t>
   </si>
@@ -190,6 +190,21 @@
   </si>
   <si>
     <t>CD274</t>
+  </si>
+  <si>
+    <t>ZFP36</t>
+  </si>
+  <si>
+    <t>IFIT1</t>
+  </si>
+  <si>
+    <t>GZMK</t>
+  </si>
+  <si>
+    <t>IFNG</t>
+  </si>
+  <si>
+    <t>LAG3</t>
   </si>
 </sst>
 </file>
@@ -535,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,6 +838,46 @@
         <v>48</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>